<commit_message>
gemini api key streamlit
</commit_message>
<xml_diff>
--- a/analyzed_results.xlsx
+++ b/analyzed_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,47 +482,47 @@
       <c r="B2" t="inlineStr">
         <is>
           <t>[2023-01-01]
-内膜組織診の結果、体部類内膜癌、Stage IAと診断。 糖尿病（HbA1c 8.8%）あり
-[2023-01-12]
-治療方針：腹腔鏡下子宮全摘の方針。
-[2023-01-29]
-手術記録：腹腔鏡下子宮全摘施行。手術時間325分、出血量514ml。
-[2023-02-08]
-術後化学療法としてDCを開始。
-[2023-02-25]
-術後化学療法としてPTX+CBDCAを開始。
-[2023-03-10]
-術後化学療法としてDC療法を開始。</t>
+内膜組織診の結果、漿液性卵巣癌、Stage IIIAと診断。 抗凝固薬（エリキュース）服用中
+[2023-01-26]
+治療方針：腹腔鏡下子宮全摘+両側付属器切除術の方針。 腎機能低下（Cr 1.9 mg/dl）
+[2023-02-20]
+手術記録：腹腔鏡下子宮全摘施行。手術時間242分、出血量275ml。
+[2023-03-15]
+術後化学療法としてパクリタキセル+カルボプラチンを開始。
+[2023-03-24]
+術後化学療法としてweekly PTXを開始。
+[2023-04-15]
+術後化学療法としてPTX+CBDCAを開始。</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>子宮体部類内膜癌</t>
+          <t>漿液性卵巣癌</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-01-01のカルテに記載された最新の診断名</t>
+          <t>カルテ1行目に記載された最新の診断名</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Stage IA</t>
+          <t>Stage IIIA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-01-01の内膜組織診の結果に記載された確定ステージ</t>
+          <t>2023-01-01のカルテに記載された最新のステージ情報</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>内膜組織診: 体部類内膜癌、Stage IA</t>
+          <t>2023/01/01 内膜組織診: 漿液性卵巣癌、Stage IIIA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2023-01-01の記載より、内膜組織診の結果が体部類内膜癌、Stage IAと診断されているため</t>
+          <t>2023-01-01の記載から内膜組織診の結果が抽出されました。</t>
         </is>
       </c>
     </row>
@@ -533,49 +533,98 @@
       <c r="B3" t="inlineStr">
         <is>
           <t>[2023-01-01]
-内膜組織診の結果、子宮体部癌、Stage ICと診断。
-[2023-01-23]
-治療方針：開腹子宮摘出術の方針。
-[2023-01-30]
-手術記録：開腹子宮全摘施行。手術時間217分、出血量143ml。
-[2023-02-15]
-術後化学療法としてDTX+CBDCAを開始。
+組織診断の結果、卵巣腫瘍、Stage IICと診断。 高度肥満（BMI 36.2）
+[2023-01-22]
+治療方針：開腹子宮全摘出術の方針。
+[2023-02-11]
+手術記録：腹腔鏡下子宮全摘施行。手術時間255分、出血量853ml。
+[2023-03-04]
+術後化学療法としてドセタキセル+カルボプラチンを開始。
+[2023-04-02]
+術後化学療法としてドセタキセル+カルボプラチンを開始。</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>{"result": "卵巣腫瘍", "reason": "2023-01-01のカルテに記載された最新の診断名"}
+ただし、"卵巣腫瘍"はがんの具体的な診断名とは言えません。病理診断などで具体的な組織型が記載されていないため、より具体的な診断名が見つからなかった場合、以下のように出力します。
+{"result": "記載なし", "reason": "がんの具体的な診断名の記載が見つかりませんでした"}</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>JSONエラー</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Stage IIC</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-01-01の組織診断結果に記載された最新のステージ情報</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2023/02/11 腹腔鏡下子宮全摘施行</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2023-02-11の手術記録から抽出</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>[2023-01-01]
+組織診断の結果、卵巣癌、Stage IBと診断。
+[2023-01-09]
+治療方針：腹腔鏡下全摘術の方針。 抗凝固薬（イグザレルト）服用中
+[2023-02-03]
+手術記録：開腹子宮全摘出術施行。手術時間226分、出血量72ml。
 [2023-03-03]
-術後化学療法として毎週パクリタキセルを開始。
-[2023-03-13]
-術後化学療法としてweekly PTXを開始。
-[2023-04-05]
-術後化学療法として毎週パクリタキセルを開始。</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>子宮体部癌</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
+術後化学療法としてドセタキセル+カルボプラチンを開始。
+[2023-03-30]
+術後化学療法としてTC療法を開始。
+[2023-04-29]
+術後化学療法としてweekly パクリタキセルを開始。 心機能低下（EF 47%）あり</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>卵巣癌</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>2023-01-01のカルテに記載された最新の診断名</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Stage IC</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2023-01-01の内膜組織診の結果に記載された最新のステージ情報</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>子宮体部癌、Stage IC (内膜組織診)</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2023-01-01の記載より、内膜組織診の結果が子宮体部癌、Stage ICと診断されているため。</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Stage IB</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2023-01-01の組織診断の結果に記載された最新のステージ情報</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2023/02/03 開腹子宮全摘出術</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2023-02-03の手術記録から抽出</t>
         </is>
       </c>
     </row>

</xml_diff>